<commit_message>
Various updates for new data
Add updated data and account for new edge cases/odd formats
</commit_message>
<xml_diff>
--- a/input/named_variants.xlsx
+++ b/input/named_variants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanta\Dropbox\PC (2)\Documents\geospatial-lineages-project\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4773F4D-1061-4FFB-9BB1-5025FF754C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597E062B-4EFF-450F-9C1A-8E34C4EB448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{89DF1878-07F4-4C66-94F9-E0CA6E807DCB}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{89DF1878-07F4-4C66-94F9-E0CA6E807DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="108">
   <si>
     <t>B.1.1.529</t>
   </si>
@@ -107,15 +107,6 @@
     <t>Delta</t>
   </si>
   <si>
-    <t>XBB.1.9.1</t>
-  </si>
-  <si>
-    <t>XBB.1.9.2</t>
-  </si>
-  <si>
-    <t>XBB.2.3</t>
-  </si>
-  <si>
     <t>XBB.1.16</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>CH.1.1</t>
   </si>
   <si>
-    <t>BA.2.74</t>
-  </si>
-  <si>
     <t>BA.2.86</t>
   </si>
   <si>
@@ -167,18 +155,9 @@
     <t>B.1.621</t>
   </si>
   <si>
-    <t>B.1.621.1</t>
-  </si>
-  <si>
     <t>Mu</t>
   </si>
   <si>
-    <t>B.1.1.529.2.75.3.4.1.1.1</t>
-  </si>
-  <si>
-    <t>B.1.1.529.2.74</t>
-  </si>
-  <si>
     <t>B.1.1.529.2.86</t>
   </si>
   <si>
@@ -194,12 +173,6 @@
     <t>AY</t>
   </si>
   <si>
-    <t>EG</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
     <t>lineage_id</t>
   </si>
   <si>
@@ -207,6 +180,186 @@
   </si>
   <si>
     <t>alias_id</t>
+  </si>
+  <si>
+    <t>highest_status</t>
+  </si>
+  <si>
+    <t>B.1.1.519</t>
+  </si>
+  <si>
+    <t>VUM</t>
+  </si>
+  <si>
+    <t>VOC</t>
+  </si>
+  <si>
+    <t>B.1.1.482.1</t>
+  </si>
+  <si>
+    <t>AV.1</t>
+  </si>
+  <si>
+    <t>B.1.617.3</t>
+  </si>
+  <si>
+    <t>VOI</t>
+  </si>
+  <si>
+    <t>B.1.1.37</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>C.37</t>
+  </si>
+  <si>
+    <t>CAL.20C</t>
+  </si>
+  <si>
+    <t>B.1.616</t>
+  </si>
+  <si>
+    <t>C.1.2</t>
+  </si>
+  <si>
+    <t>B.1.1.1.1.7</t>
+  </si>
+  <si>
+    <t>B.1.1.28.3</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>P.3</t>
+  </si>
+  <si>
+    <t>B.1.214.2</t>
+  </si>
+  <si>
+    <t>A.27</t>
+  </si>
+  <si>
+    <t>A.28</t>
+  </si>
+  <si>
+    <t>C.16</t>
+  </si>
+  <si>
+    <t>B.1.1.1.16</t>
+  </si>
+  <si>
+    <t>B.1.526.1</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>B.1.620</t>
+  </si>
+  <si>
+    <t>B.1.1.370.1</t>
+  </si>
+  <si>
+    <t>AT.1</t>
+  </si>
+  <si>
+    <t>B.1.617.2.4.2</t>
+  </si>
+  <si>
+    <t>AY.4.2</t>
+  </si>
+  <si>
+    <t>B.1.640</t>
+  </si>
+  <si>
+    <t>B.1.1.318</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>XF</t>
+  </si>
+  <si>
+    <t>BA.2.75</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.75</t>
+  </si>
+  <si>
+    <t>XAK</t>
+  </si>
+  <si>
+    <t>B.1.1.529.5.3.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>BQ.1</t>
+  </si>
+  <si>
+    <t>XBB</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.30</t>
+  </si>
+  <si>
+    <t>BA.2.30</t>
+  </si>
+  <si>
+    <t>B.1.1.529.5.2.1.7</t>
+  </si>
+  <si>
+    <t>BF.7</t>
+  </si>
+  <si>
+    <t>XBC</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.75.5.1</t>
+  </si>
+  <si>
+    <t>BN.1</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.75.3.4.1.1.1.1</t>
+  </si>
+  <si>
+    <t>XAY</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.3.20</t>
+  </si>
+  <si>
+    <t>BA.2.3.20</t>
+  </si>
+  <si>
+    <t>XBB.1.18.1.1</t>
+  </si>
+  <si>
+    <t>FE.1</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.75.3.4.1.1.1.1.1.7.1</t>
+  </si>
+  <si>
+    <t>DV.7.1</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.87.1</t>
+  </si>
+  <si>
+    <t>BA.2.87.1</t>
+  </si>
+  <si>
+    <t>B.1.1.529.2.86.1.1.11.1.3</t>
+  </si>
+  <si>
+    <t>KP.3</t>
+  </si>
+  <si>
+    <t>XEC</t>
   </si>
 </sst>
 </file>
@@ -248,8 +401,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,325 +718,816 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1046998-B463-4A61-ADB0-CB62F8DD792D}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
       <c r="C22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-    </row>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>